<commit_message>
added tests for cytof_analysis_template
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CFD53D-3695-F841-9528-C2C76FC5626B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCAB46E-E326-1443-ACE0-FCDDDB5555A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -226,9 +226,6 @@
     <t>Cell counts profiling</t>
   </si>
   <si>
-    <t>CPPPTTTNN.00</t>
-  </si>
-  <si>
     <t>fcs.fcs</t>
   </si>
   <si>
@@ -257,13 +254,16 @@
   </si>
   <si>
     <t>test_trial_1</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +289,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -356,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -367,6 +373,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +715,7 @@
   <dimension ref="A1:K205"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -742,7 +749,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -806,35 +813,35 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>25</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added assay_run_id property to cytof
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCAB46E-E326-1443-ACE0-FCDDDB5555A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7F76B7-8599-DE48-A580-8A7EC3886DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="21760" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CyTOF Analysis" sheetId="1" r:id="rId1"/>
@@ -34,16 +34,29 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>User defined unique identifier for this assay run.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -51,20 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a user's computer.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -116,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path to a file on a user's computer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -173,10 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="28">
-  <si>
-    <t>#t</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="29">
   <si>
     <t>Cytof analysis template</t>
   </si>
@@ -184,6 +194,9 @@
     <t>#p</t>
   </si>
   <si>
+    <t>Assay run id</t>
+  </si>
+  <si>
     <t>Protocol identifier</t>
   </si>
   <si>
@@ -226,6 +239,9 @@
     <t>Cell counts profiling</t>
   </si>
   <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
     <t>fcs.fcs</t>
   </si>
   <si>
@@ -238,32 +254,32 @@
     <t>assignment.csv</t>
   </si>
   <si>
-    <t>compar.csv</t>
+    <t>comp.csv</t>
   </si>
   <si>
     <t>profiling.csv</t>
   </si>
   <si>
-    <t>csa.csv</t>
-  </si>
-  <si>
-    <t>csc.csv</t>
-  </si>
-  <si>
-    <t>csp.csv</t>
+    <t>cca.csv</t>
+  </si>
+  <si>
+    <t>ccc.csv</t>
+  </si>
+  <si>
+    <t>ccp.csv</t>
   </si>
   <si>
     <t>test_trial_1</t>
   </si>
   <si>
-    <t>CTTTPP111.00</t>
+    <t>run_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,12 +298,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -373,7 +383,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K205"/>
+  <dimension ref="A1:K206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -725,11 +735,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -743,13 +753,13 @@
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -760,94 +770,108 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1836,13 +1860,18 @@
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
update cytof xlsx templates
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4314C4F6-34A6-5B4A-8EA7-28837C7B51E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD6DEAD-8995-1D48-AF28-65CA4A68D79B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="21760" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CyTOF Analysis" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
     <t>run_1</t>
   </si>
   <si>
-    <t>CYTOF_ANALYSIS_TEST1</t>
+    <t>CYTOF_TEST1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Converge on test_prism_trial_id as the example template protocol identifier
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD6DEAD-8995-1D48-AF28-65CA4A68D79B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB45500-7F6D-6449-90D7-C692DDFF6912}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CyTOF Analysis" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
     <t>run_1</t>
   </si>
   <si>
-    <t>CYTOF_TEST1</t>
+    <t>test_prism_trial_id</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
assay_run_date introduced to all assays
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508DE28D-1748-F047-98B9-5773544B2E86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55FE6EB-8411-5243-88E9-B03099366BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -186,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="28">
   <si>
     <t>Cytof analysis template</t>
   </si>
@@ -194,9 +194,6 @@
     <t>#p</t>
   </si>
   <si>
-    <t>Assay run id</t>
-  </si>
-  <si>
     <t>Protocol identifier</t>
   </si>
   <si>
@@ -272,14 +269,14 @@
     <t>test_prism_trial_id</t>
   </si>
   <si>
-    <t>test_prism_trial_id_run_1</t>
+    <t>Assay run date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +311,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -386,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -400,6 +403,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,7 +748,7 @@
   <dimension ref="A1:K206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -753,7 +759,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -773,10 +779,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C2" s="6">
+        <v>36892</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -792,10 +798,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -808,7 +814,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -822,1067 +828,1067 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>23</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>25</v>
-      </c>
-      <c r="K7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update gcs uri of sample level analyses
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E0EFFC-402C-7443-9244-30D3D17947E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4C2E8A-5530-1145-BCB4-4D80BBADF836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11220" yWindow="2620" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,12 +112,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.
-In .fcs format</t>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
         </r>
       </text>
     </comment>
@@ -210,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="51">
   <si>
     <t>#t</t>
   </si>
@@ -308,41 +317,68 @@
     <t>test_prism_trial_id</t>
   </si>
   <si>
-    <t>reports.zip</t>
-  </si>
-  <si>
-    <t>analysis.zip</t>
-  </si>
-  <si>
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>fcs.fcs</t>
-  </si>
-  <si>
-    <t>assignment.csv</t>
-  </si>
-  <si>
-    <t>comp.csv</t>
-  </si>
-  <si>
-    <t>profiling.csv</t>
-  </si>
-  <si>
-    <t>cca.csv</t>
-  </si>
-  <si>
-    <t>ccc.csv</t>
-  </si>
-  <si>
-    <t>ccp.csv</t>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00/fcs.fcs</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00/assignment.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00/comp.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00/profiling.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00/cca.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00/ccc.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00/ccp.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00/fcs.fcs</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00/assignment.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00/comp.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00/profiling.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00/cca.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00/ccc.csv</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00/ccp.csv</t>
+  </si>
+  <si>
+    <t>batch1/reports.zip</t>
+  </si>
+  <si>
+    <t>batch1/analysis.zip</t>
+  </si>
+  <si>
+    <t>XYZ1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +397,19 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -435,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -449,6 +498,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -793,7 +843,7 @@
   <dimension ref="A1:I209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -806,16 +856,16 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -858,8 +908,8 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
+      <c r="C4" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -876,7 +926,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -893,7 +943,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -903,16 +953,16 @@
       <c r="I6" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -948,33 +998,57 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>38</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>39</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>40</v>
-      </c>
-      <c r="I10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Set service column width
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -613,7 +613,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col hidden="1" min="1" max="1"/>
+    <col hidden="1" width="30" customWidth="1" min="1" max="1"/>
     <col width="30.6640625" customWidth="1" min="2" max="101"/>
   </cols>
   <sheetData>
@@ -751,7 +751,6 @@
       <c r="H6" s="2" t="n"/>
       <c r="I6" s="2" t="n"/>
     </row>
-    <row r="7"/>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
@@ -2314,7 +2313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2322,6 +2321,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
     <col width="30.6640625" customWidth="1" min="2" max="101"/>
   </cols>
   <sheetData>
@@ -2591,6 +2591,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
     <col width="30.6640625" customWidth="1" min="2" max="101"/>
   </cols>
   <sheetData/>

</xml_diff>

<commit_message>
add control_files_analysis; regenerate documentation
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D222B923-1DF1-C244-966C-869043B76776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9ED18C-B524-2640-A721-E79782162AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CyTOF Analysis" sheetId="1" r:id="rId1"/>
@@ -895,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2010"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -11085,7 +11085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
add excluded samples tab
</commit_message>
<xml_diff>
--- a/template_examples/cytof_analysis_template.xlsx
+++ b/template_examples/cytof_analysis_template.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9ED18C-B524-2640-A721-E79782162AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E162D08-BFA6-AE46-8A3F-0D04178E247A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CyTOF Analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Legend" sheetId="3" r:id="rId2"/>
-    <sheet name="Data Dictionary" sheetId="4" r:id="rId3"/>
+    <sheet name="Excluded Samples" sheetId="5" r:id="rId2"/>
+    <sheet name="Legend" sheetId="3" r:id="rId3"/>
+    <sheet name="Data Dictionary" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -232,8 +233,44 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>CIDC</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{B9CBE9FE-313A-1545-AE1F-A46D5C395062}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{5EFD4EE3-1183-1A43-B7EB-1977CB4F1711}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A comment describing why this sample is missing from the pipeline output.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="62">
   <si>
     <t>LEGEND</t>
   </si>
@@ -408,6 +445,18 @@
   <si>
     <t>batch1/control_files_analysis.zip</t>
   </si>
+  <si>
+    <t>Samples Excluded From Analysis</t>
+  </si>
+  <si>
+    <t>low coverage</t>
+  </si>
+  <si>
+    <t>CTTTPP122.00</t>
+  </si>
+  <si>
+    <t>module failed</t>
+  </si>
 </sst>
 </file>
 
@@ -535,7 +584,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -553,6 +602,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,7 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -11082,6 +11133,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8AA65F-E850-8348-A215-7EC4C6D1CAF8}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:E21"/>
   <sheetViews>
@@ -11305,7 +11421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>